<commit_message>
enviando email via chamada api, sem passagem de parametros
</commit_message>
<xml_diff>
--- a/backend/code/relatorios/tabelaPedidos.xlsx
+++ b/backend/code/relatorios/tabelaPedidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,58 +491,62 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>28/04/2021</t>
+          <t>03/05/2021</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>09:13</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>51</v>
+        <v>8.555</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cartão</t>
+          <t>Dinheiro</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>27/04/2021</t>
+          <t>03/05/2021</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>23:09</t>
+          <t>21:25</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>53</v>
+        <v>13.055</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Dinheiro</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>27/04/2021</t>
+          <t>28/04/2021</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>20:38</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>17.11</v>
+        <v>51</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -551,7 +555,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Dinheiro</t>
+          <t>Cartão</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -561,13 +565,124 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>23:11</t>
+          <t>23:09</t>
         </is>
       </c>
       <c r="D6" t="n">
         <v>53</v>
       </c>
       <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Cartão</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>02/05/2021</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>22:36</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>8.555</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Cartão</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>02/05/2021</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>19:56</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>60</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Cartão</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>02/05/2021</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>160</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>27/04/2021</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>20:38</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>17.11</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Dinheiro</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>27/04/2021</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>23:11</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>53</v>
+      </c>
+      <c r="E11" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>